<commit_message>
Visual Overhaul to reduce headache color scheme
</commit_message>
<xml_diff>
--- a/data/Algemene informatie.xlsx
+++ b/data/Algemene informatie.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
   <si>
     <t>1 day = 24 hours</t>
   </si>
@@ -238,6 +238,1139 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <r>
+      <t>smAxis = (OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) / 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitVelocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = sqrt[μ / OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Velocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = sqrt[μ * ((2 / OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) - (1 / smAxis))]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DeltaV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = Velocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - OrbitVelocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitVelocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = sqrt[μ / OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Velocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = sqrt[μ * ((2 / OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) - (1 / smAxis))]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DeltaV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = Velocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - OrbitVelocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+  </si>
+  <si>
+    <t>with:</t>
+  </si>
+  <si>
+    <r>
+      <t>OrbitVelocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = orbital velocity of the starting planet (m/s), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i.e.,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> free delta V</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Velocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = velocity needed for Insertion Burn (m/s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitVelocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = orbital velocity of the destination planet (m/s), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i.e.,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> free delta V</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Velocity</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = velocity needed for Arrival Burn (m/s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DeltaV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = actual total delta V needed for the entire Hohmann transfer, which is what you were doing all these calculations for in the first place</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DeltaV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = abs[DeltaV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>] + abs[DeltaV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DeltaV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = actual delta V needed for Arrival Burn (m/s) after taking advantage of the free delta v</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DeltaV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = actual delta V needed for Insertion Burn (m/s) after taking advantage of the free delta v</t>
+    </r>
+  </si>
+  <si>
+    <t>1 - Delta V:</t>
+  </si>
+  <si>
+    <t>2 - Transit time:</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.5 * sqrt[(4 * π</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> * smAxis</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) / μ]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = orbital radius of starting planet (m)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) = orbital radius of destination planet (m)</t>
+    </r>
+  </si>
+  <si>
+    <t>μ = solar gravitational constant (see above)</t>
+  </si>
+  <si>
+    <t>smAxis = Semi-major axis of Hohmann Transfer orbit (meters)</t>
+  </si>
+  <si>
+    <t>smAxis = see above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transit time is in seconds! </t>
+  </si>
+  <si>
+    <t>1 day = 24 * 3600 = 86400 secs</t>
+  </si>
+  <si>
+    <t>3 - Hohmann Launch Windows</t>
+  </si>
+  <si>
+    <r>
+      <t>OrbitPeriod</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 2 * π * sqrt[OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / μ]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitPeriod</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 2 * π * sqrt[OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / μ]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SynodicPeriod = 1 / ( (1/OrbitPeriod</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) - (1/OrbitPeriod</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>SynodicPeriod = time delay between Hohmann launch windows (seconds)</t>
+  </si>
+  <si>
+    <r>
+      <t>OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = orbital radius of planet closer to central object (meters)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = orbital radius of planet further away from central object (meters)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitPeriod</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = one planetary year for the inferior planet (seconds)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitPeriod</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = one planetary year for the superior planet (seconds)</t>
+    </r>
+  </si>
+  <si>
+    <t>Convert radians into decimal degrees by muliplying by (180/π), which is approximately 57.29578...</t>
+  </si>
+  <si>
+    <t>4 - Calculate launch timing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">α = π * (1 - ( </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.35355</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> * sqrt[(OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 1)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">α = Phase Angle, or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>angle StartPlanet-CenterObject-DestPlanet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (radians). If negative, DestPlanet is behind StarPlanet, otherwise it is ahead.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = orbital radius of start planet (meters)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OrbitRadius</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = orbital radius of destination planet (meters)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -247,7 +1380,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -264,6 +1397,33 @@
     <font>
       <b/>
       <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -405,7 +1565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -471,6 +1631,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q61"/>
+  <dimension ref="B2:Q107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1266,598 +2430,909 @@
       </c>
     </row>
     <row r="32" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C33" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="3:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="1" t="s">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C35" s="18"/>
+      <c r="D35" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+    </row>
+    <row r="36" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C36" s="18"/>
+      <c r="D36" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+    </row>
+    <row r="37" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C37" s="18"/>
+      <c r="D37" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+    </row>
+    <row r="38" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C38" s="18"/>
+      <c r="D38" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+    </row>
+    <row r="39" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C39" s="18"/>
+      <c r="D39" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+    </row>
+    <row r="40" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C40" s="18"/>
+      <c r="D40" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+    </row>
+    <row r="41" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C41" s="18"/>
+      <c r="D41" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+    </row>
+    <row r="42" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C42" s="18"/>
+      <c r="D42" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C43" s="18"/>
+      <c r="D43" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C44" s="18"/>
+      <c r="D44" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C45" s="18"/>
+      <c r="D45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+    </row>
+    <row r="46" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C46" s="18"/>
+      <c r="D46" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+    </row>
+    <row r="47" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C47" s="18"/>
+      <c r="D47" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+    </row>
+    <row r="48" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C48" s="18"/>
+      <c r="D48" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C49" s="18"/>
+      <c r="D49" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C50" s="18"/>
+      <c r="D50" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C51" s="18"/>
+      <c r="D51" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C52" s="18"/>
+      <c r="D52" s="33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C53" s="18"/>
+      <c r="D53" s="33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="18"/>
+      <c r="D54" s="33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="33"/>
+    </row>
+    <row r="56" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C56" s="1"/>
+      <c r="D56" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="1"/>
+      <c r="D57" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C58" s="1"/>
+      <c r="D58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C59" s="1"/>
+      <c r="D59" s="33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C60" s="1"/>
+      <c r="D60" s="33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C61" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" s="33"/>
+    </row>
+    <row r="62" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C62" s="1"/>
+      <c r="D62" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C63" s="1"/>
+      <c r="D63" s="33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C64" s="1"/>
+      <c r="D64" s="33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C65" s="1"/>
+      <c r="D65" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="1"/>
+      <c r="D66" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C67" s="1"/>
+      <c r="D67" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C68" s="1"/>
+      <c r="D68" s="33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C69" s="1"/>
+      <c r="D69" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C70" s="1"/>
+      <c r="D70" s="33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C71" s="1"/>
+      <c r="D71" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="33"/>
+    </row>
+    <row r="73" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C73" s="1"/>
+      <c r="D73" s="33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C74" s="18"/>
+      <c r="D74" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C75" s="18"/>
+      <c r="D75" s="33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C76" s="18"/>
+      <c r="D76" s="33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C77" s="18"/>
+      <c r="D77" s="33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C78" s="18"/>
+      <c r="D78" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C79" s="18"/>
+    </row>
+    <row r="81" spans="4:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D36" s="20"/>
-      <c r="E36" s="21" t="s">
+    <row r="82" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D82" s="20"/>
+      <c r="E82" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F82" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G82" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H36" s="21" t="s">
+      <c r="H82" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="21" t="s">
+      <c r="I82" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J36" s="21" t="s">
+      <c r="J82" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="21" t="s">
+      <c r="K82" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L36" s="21" t="s">
+      <c r="L82" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="M36" s="21" t="s">
+      <c r="M82" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N36" s="21" t="s">
+      <c r="N82" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="O36" s="22" t="s">
+      <c r="O82" s="22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D37" s="23" t="s">
+    <row r="83" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D83" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="24">
+      <c r="E83" s="24">
         <v>9.6633782422689762</v>
       </c>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-    </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D38" s="23" t="s">
+      <c r="F83" s="25"/>
+      <c r="G83" s="25"/>
+      <c r="H83" s="25"/>
+      <c r="I83" s="25"/>
+      <c r="J83" s="25"/>
+      <c r="K83" s="25"/>
+      <c r="L83" s="25"/>
+      <c r="M83" s="25"/>
+      <c r="N83" s="25"/>
+      <c r="O83" s="26"/>
+      <c r="P83" s="19"/>
+      <c r="Q83" s="19"/>
+    </row>
+    <row r="84" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D84" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E84" s="24">
         <v>21.400925684871464</v>
       </c>
-      <c r="F38" s="24">
+      <c r="F84" s="24">
         <v>12.637702235618857</v>
       </c>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-    </row>
-    <row r="39" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D39" s="23" t="s">
+      <c r="G84" s="25"/>
+      <c r="H84" s="25"/>
+      <c r="I84" s="25"/>
+      <c r="J84" s="25"/>
+      <c r="K84" s="25"/>
+      <c r="L84" s="25"/>
+      <c r="M84" s="25"/>
+      <c r="N84" s="25"/>
+      <c r="O84" s="26"/>
+      <c r="P84" s="19"/>
+      <c r="Q84" s="19"/>
+    </row>
+    <row r="85" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D85" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E85" s="24">
         <v>25.754233035534071</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F85" s="24">
         <v>17.784331331029652</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G85" s="24">
         <v>5.8586340519109363</v>
       </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
-    </row>
-    <row r="40" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D40" s="23" t="s">
+      <c r="H85" s="25"/>
+      <c r="I85" s="25"/>
+      <c r="J85" s="25"/>
+      <c r="K85" s="25"/>
+      <c r="L85" s="25"/>
+      <c r="M85" s="25"/>
+      <c r="N85" s="25"/>
+      <c r="O85" s="26"/>
+      <c r="P85" s="19"/>
+      <c r="Q85" s="19"/>
+    </row>
+    <row r="86" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D86" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E86" s="24">
         <v>28.533294867616132</v>
       </c>
-      <c r="F40" s="24">
+      <c r="F86" s="24">
         <v>21.358149299295999</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G86" s="24">
         <v>10.405895392915248</v>
       </c>
-      <c r="H40" s="24">
+      <c r="H86" s="24">
         <v>4.798481233688177</v>
       </c>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
-    </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D41" s="23" t="s">
+      <c r="I86" s="25"/>
+      <c r="J86" s="25"/>
+      <c r="K86" s="25"/>
+      <c r="L86" s="25"/>
+      <c r="M86" s="25"/>
+      <c r="N86" s="25"/>
+      <c r="O86" s="26"/>
+      <c r="P86" s="19"/>
+      <c r="Q86" s="19"/>
+    </row>
+    <row r="87" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D87" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E87" s="24">
         <v>30.209531091799239</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F87" s="24">
         <v>23.791666070248962</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G87" s="24">
         <v>13.950143670758971</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H87" s="24">
         <v>8.7812443920451813</v>
       </c>
-      <c r="I41" s="24">
+      <c r="I87" s="24">
         <v>4.2026232601901139</v>
       </c>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-    </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D42" s="23" t="s">
+      <c r="J87" s="25"/>
+      <c r="K87" s="25"/>
+      <c r="L87" s="25"/>
+      <c r="M87" s="25"/>
+      <c r="N87" s="25"/>
+      <c r="O87" s="26"/>
+      <c r="P87" s="19"/>
+      <c r="Q87" s="19"/>
+    </row>
+    <row r="88" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D88" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E88" s="24">
         <v>30.98982890824842</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F88" s="24">
         <v>25.266360588697768</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G88" s="24">
         <v>16.581434892160861</v>
       </c>
-      <c r="H42" s="24">
+      <c r="H88" s="24">
         <v>11.984674949378961</v>
       </c>
-      <c r="I42" s="24">
+      <c r="I88" s="24">
         <v>7.8192402272642161</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J88" s="24">
         <v>3.8477009450201529</v>
       </c>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="26"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-    </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D43" s="23" t="s">
+      <c r="K88" s="25"/>
+      <c r="L88" s="25"/>
+      <c r="M88" s="25"/>
+      <c r="N88" s="25"/>
+      <c r="O88" s="26"/>
+      <c r="P88" s="19"/>
+      <c r="Q88" s="19"/>
+    </row>
+    <row r="89" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D89" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="24">
+      <c r="E89" s="24">
         <v>31.045629834410079</v>
       </c>
-      <c r="F43" s="24">
+      <c r="F89" s="24">
         <v>25.768878632462879</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G89" s="24">
         <v>17.894057950142287</v>
       </c>
-      <c r="H43" s="24">
+      <c r="H89" s="24">
         <v>13.75601659146623</v>
       </c>
-      <c r="I43" s="24">
+      <c r="I89" s="24">
         <v>9.9825492802326181</v>
       </c>
-      <c r="J43" s="24">
+      <c r="J89" s="24">
         <v>6.3175588635757052</v>
       </c>
-      <c r="K43" s="24">
+      <c r="K89" s="24">
         <v>2.642843309595468</v>
       </c>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="26"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-    </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D44" s="23" t="s">
+      <c r="L89" s="25"/>
+      <c r="M89" s="25"/>
+      <c r="N89" s="25"/>
+      <c r="O89" s="26"/>
+      <c r="P89" s="19"/>
+      <c r="Q89" s="19"/>
+    </row>
+    <row r="90" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D90" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="24">
+      <c r="E90" s="24">
         <v>30.431995049237099</v>
       </c>
-      <c r="F44" s="24">
+      <c r="F90" s="24">
         <v>25.686686538228859</v>
       </c>
-      <c r="G44" s="24">
+      <c r="G90" s="24">
         <v>18.841440569418928</v>
       </c>
-      <c r="H44" s="24">
+      <c r="H90" s="24">
         <v>15.348688192612414</v>
       </c>
-      <c r="I44" s="24">
+      <c r="I90" s="24">
         <v>12.195634471253092</v>
       </c>
-      <c r="J44" s="24">
+      <c r="J90" s="24">
         <v>9.1163082444208197</v>
       </c>
-      <c r="K44" s="24">
+      <c r="K90" s="24">
         <v>5.9386584727886431</v>
       </c>
-      <c r="L44" s="24">
+      <c r="L90" s="24">
         <v>3.5318094602466901</v>
       </c>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="26"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-    </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D45" s="23" t="s">
+      <c r="M90" s="25"/>
+      <c r="N90" s="25"/>
+      <c r="O90" s="26"/>
+      <c r="P90" s="19"/>
+      <c r="Q90" s="19"/>
+    </row>
+    <row r="91" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D91" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="24">
+      <c r="E91" s="24">
         <v>29.78418742410155</v>
       </c>
-      <c r="F45" s="24">
+      <c r="F91" s="24">
         <v>25.266131084860184</v>
       </c>
-      <c r="G45" s="24">
+      <c r="G91" s="24">
         <v>18.882845006720498</v>
       </c>
-      <c r="H45" s="24">
+      <c r="H91" s="24">
         <v>15.701258024602081</v>
       </c>
-      <c r="I45" s="24">
+      <c r="I91" s="24">
         <v>12.872593622780521</v>
       </c>
-      <c r="J45" s="24">
+      <c r="J91" s="24">
         <v>10.137944016838757</v>
       </c>
-      <c r="K45" s="24">
+      <c r="K91" s="24">
         <v>7.3169022020680483</v>
       </c>
-      <c r="L45" s="24">
+      <c r="L91" s="24">
         <v>5.150699399104731</v>
       </c>
-      <c r="M45" s="24">
+      <c r="M91" s="24">
         <v>1.8436590686291947</v>
       </c>
-      <c r="N45" s="25"/>
-      <c r="O45" s="26"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-    </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="D46" s="23" t="s">
+      <c r="N91" s="25"/>
+      <c r="O91" s="26"/>
+      <c r="P91" s="19"/>
+      <c r="Q91" s="19"/>
+    </row>
+    <row r="92" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D92" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="24">
+      <c r="E92" s="24">
         <v>29.006262151561785</v>
       </c>
-      <c r="F46" s="24">
+      <c r="F92" s="24">
         <v>24.658207941594434</v>
       </c>
-      <c r="G46" s="24">
+      <c r="G92" s="24">
         <v>18.62900283765368</v>
       </c>
-      <c r="H46" s="24">
+      <c r="H92" s="24">
         <v>15.694768894247733</v>
       </c>
-      <c r="I46" s="24">
+      <c r="I92" s="24">
         <v>13.134837390044382</v>
       </c>
-      <c r="J46" s="24">
+      <c r="J92" s="24">
         <v>10.703363249052584</v>
       </c>
-      <c r="K46" s="24">
+      <c r="K92" s="24">
         <v>8.2275258362869739</v>
       </c>
-      <c r="L46" s="24">
+      <c r="L92" s="24">
         <v>6.3297980550911461</v>
       </c>
-      <c r="M46" s="24">
+      <c r="M92" s="24">
         <v>3.3730091454479334</v>
       </c>
-      <c r="N46" s="24">
+      <c r="N92" s="24">
         <v>1.6419645976584742</v>
       </c>
-      <c r="O46" s="26"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
-    </row>
-    <row r="47" spans="3:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="27" t="s">
+      <c r="O92" s="26"/>
+      <c r="P92" s="19"/>
+      <c r="Q92" s="19"/>
+    </row>
+    <row r="93" spans="4:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D93" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E47" s="28">
+      <c r="E93" s="28">
         <v>28.325266459893406</v>
       </c>
-      <c r="F47" s="28">
+      <c r="F93" s="28">
         <v>24.078603821677863</v>
       </c>
-      <c r="G47" s="28">
+      <c r="G93" s="28">
         <v>18.264046035514205</v>
       </c>
-      <c r="H47" s="28">
+      <c r="H93" s="28">
         <v>15.483465532843043</v>
       </c>
-      <c r="I47" s="28">
+      <c r="I93" s="28">
         <v>13.095167543212222</v>
       </c>
-      <c r="J47" s="28">
+      <c r="J93" s="28">
         <v>10.865281035266262</v>
       </c>
-      <c r="K47" s="28">
+      <c r="K93" s="28">
         <v>8.6340649167277128</v>
       </c>
-      <c r="L47" s="28">
+      <c r="L93" s="28">
         <v>6.9444827419874491</v>
       </c>
-      <c r="M47" s="28">
+      <c r="M93" s="28">
         <v>4.3131534459687284</v>
       </c>
-      <c r="N47" s="28">
+      <c r="N93" s="28">
         <v>2.739674074119018</v>
       </c>
-      <c r="O47" s="29">
+      <c r="O93" s="29">
         <v>1.1873883053578129</v>
       </c>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="19"/>
-    </row>
-    <row r="49" spans="4:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
+      <c r="P93" s="19"/>
+      <c r="Q93" s="19"/>
+    </row>
+    <row r="95" spans="4:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D50" s="20"/>
-      <c r="E50" s="21" t="s">
+    <row r="96" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D96" s="20"/>
+      <c r="E96" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="F96" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="G96" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="H96" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I50" s="21" t="s">
+      <c r="I96" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J50" s="21" t="s">
+      <c r="J96" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="K50" s="21" t="s">
+      <c r="K96" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L50" s="21" t="s">
+      <c r="L96" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="M50" s="21" t="s">
+      <c r="M96" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N50" s="21" t="s">
+      <c r="N96" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="O50" s="22" t="s">
+      <c r="O96" s="22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D51" s="23" t="s">
+    <row r="97" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D97" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="24"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="25"/>
-      <c r="L51" s="25"/>
-      <c r="M51" s="25"/>
-      <c r="N51" s="25"/>
-      <c r="O51" s="26"/>
-    </row>
-    <row r="52" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D52" s="23" t="s">
+      <c r="E97" s="24"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="25"/>
+      <c r="H97" s="25"/>
+      <c r="I97" s="25"/>
+      <c r="J97" s="25"/>
+      <c r="K97" s="25"/>
+      <c r="L97" s="25"/>
+      <c r="M97" s="25"/>
+      <c r="N97" s="25"/>
+      <c r="O97" s="26"/>
+    </row>
+    <row r="98" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D98" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="26"/>
-    </row>
-    <row r="53" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D53" s="23" t="s">
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="25"/>
+      <c r="H98" s="25"/>
+      <c r="I98" s="25"/>
+      <c r="J98" s="25"/>
+      <c r="K98" s="25"/>
+      <c r="L98" s="25"/>
+      <c r="M98" s="25"/>
+      <c r="N98" s="25"/>
+      <c r="O98" s="26"/>
+    </row>
+    <row r="99" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D99" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="26"/>
-    </row>
-    <row r="54" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D54" s="23" t="s">
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24"/>
+      <c r="H99" s="25"/>
+      <c r="I99" s="25"/>
+      <c r="J99" s="25"/>
+      <c r="K99" s="25"/>
+      <c r="L99" s="25"/>
+      <c r="M99" s="25"/>
+      <c r="N99" s="25"/>
+      <c r="O99" s="26"/>
+    </row>
+    <row r="100" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D100" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="26"/>
-    </row>
-    <row r="55" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D55" s="23" t="s">
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+      <c r="I100" s="25"/>
+      <c r="J100" s="25"/>
+      <c r="K100" s="25"/>
+      <c r="L100" s="25"/>
+      <c r="M100" s="25"/>
+      <c r="N100" s="25"/>
+      <c r="O100" s="26"/>
+    </row>
+    <row r="101" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D101" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="26"/>
-    </row>
-    <row r="56" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D56" s="23" t="s">
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
+      <c r="I101" s="24"/>
+      <c r="J101" s="25"/>
+      <c r="K101" s="25"/>
+      <c r="L101" s="25"/>
+      <c r="M101" s="25"/>
+      <c r="N101" s="25"/>
+      <c r="O101" s="26"/>
+    </row>
+    <row r="102" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D102" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
-      <c r="J56" s="24"/>
-      <c r="K56" s="25"/>
-      <c r="L56" s="25"/>
-      <c r="M56" s="25"/>
-      <c r="N56" s="25"/>
-      <c r="O56" s="26"/>
-    </row>
-    <row r="57" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D57" s="23" t="s">
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="24"/>
+      <c r="K102" s="25"/>
+      <c r="L102" s="25"/>
+      <c r="M102" s="25"/>
+      <c r="N102" s="25"/>
+      <c r="O102" s="26"/>
+    </row>
+    <row r="103" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D103" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
-      <c r="K57" s="24"/>
-      <c r="L57" s="25"/>
-      <c r="M57" s="25"/>
-      <c r="N57" s="25"/>
-      <c r="O57" s="26"/>
-    </row>
-    <row r="58" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D58" s="23" t="s">
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+      <c r="I103" s="24"/>
+      <c r="J103" s="24"/>
+      <c r="K103" s="24"/>
+      <c r="L103" s="25"/>
+      <c r="M103" s="25"/>
+      <c r="N103" s="25"/>
+      <c r="O103" s="26"/>
+    </row>
+    <row r="104" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D104" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="24"/>
-      <c r="J58" s="24"/>
-      <c r="K58" s="24"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="25"/>
-      <c r="N58" s="25"/>
-      <c r="O58" s="26"/>
-    </row>
-    <row r="59" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D59" s="23" t="s">
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="24"/>
+      <c r="J104" s="24"/>
+      <c r="K104" s="24"/>
+      <c r="L104" s="24"/>
+      <c r="M104" s="25"/>
+      <c r="N104" s="25"/>
+      <c r="O104" s="26"/>
+    </row>
+    <row r="105" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D105" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="24"/>
-      <c r="J59" s="24"/>
-      <c r="K59" s="24"/>
-      <c r="L59" s="24"/>
-      <c r="M59" s="24"/>
-      <c r="N59" s="25"/>
-      <c r="O59" s="26"/>
-    </row>
-    <row r="60" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D60" s="23" t="s">
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="24"/>
+      <c r="I105" s="24"/>
+      <c r="J105" s="24"/>
+      <c r="K105" s="24"/>
+      <c r="L105" s="24"/>
+      <c r="M105" s="24"/>
+      <c r="N105" s="25"/>
+      <c r="O105" s="26"/>
+    </row>
+    <row r="106" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D106" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="24"/>
-      <c r="K60" s="24"/>
-      <c r="L60" s="24"/>
-      <c r="M60" s="24"/>
-      <c r="N60" s="24"/>
-      <c r="O60" s="26"/>
-    </row>
-    <row r="61" spans="4:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D61" s="27" t="s">
+      <c r="E106" s="24"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="24"/>
+      <c r="H106" s="24"/>
+      <c r="I106" s="24"/>
+      <c r="J106" s="24"/>
+      <c r="K106" s="24"/>
+      <c r="L106" s="24"/>
+      <c r="M106" s="24"/>
+      <c r="N106" s="24"/>
+      <c r="O106" s="26"/>
+    </row>
+    <row r="107" spans="4:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D107" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
-      <c r="J61" s="28"/>
-      <c r="K61" s="28"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="28"/>
-      <c r="N61" s="28"/>
-      <c r="O61" s="29"/>
+      <c r="E107" s="28"/>
+      <c r="F107" s="28"/>
+      <c r="G107" s="28"/>
+      <c r="H107" s="28"/>
+      <c r="I107" s="28"/>
+      <c r="J107" s="28"/>
+      <c r="K107" s="28"/>
+      <c r="L107" s="28"/>
+      <c r="M107" s="28"/>
+      <c r="N107" s="28"/>
+      <c r="O107" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Simulation works, moons included. Scale's a little off.
</commit_message>
<xml_diff>
--- a/data/Algemene informatie.xlsx
+++ b/data/Algemene informatie.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f5229ea5dc7911b/Projects/SystemSimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
   <si>
     <t>1 day = 24 hours</t>
   </si>
@@ -1371,16 +1371,20 @@
       </rPr>
       <t xml:space="preserve"> = orbital radius of destination planet (meters)</t>
     </r>
+  </si>
+  <si>
+    <t>radius (in km)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1397,12 +1401,6 @@
     <font>
       <b/>
       <vertAlign val="subscript"/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1565,7 +1563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1626,15 +1624,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1729,6 +1731,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1764,6 +1783,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1942,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1959,7 +1995,7 @@
     <col min="11" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1970,12 +2006,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -1986,7 +2022,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -1997,7 +2033,12 @@
         <v>149597870700</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J6" s="34">
+        <v>149600000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
@@ -2008,34 +2049,37 @@
         <v>53</v>
       </c>
       <c r="F7">
-        <v>1.1679885359999998E+20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="2:10" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:10" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.167988536E+20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="2:12" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="30" t="s">
+      <c r="F11" s="33"/>
+      <c r="G11" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="31"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
@@ -2058,7 +2102,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
@@ -2085,8 +2129,15 @@
         <f>360/H13</f>
         <v>8.2462849772789486</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="2">
+        <v>6371</v>
+      </c>
+      <c r="L13" s="35">
+        <f>K13/J6</f>
+        <v>4.2586898395721926E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
@@ -2113,8 +2164,15 @@
         <f t="shared" ref="J14:J24" si="1">360/H14</f>
         <v>4.746225364555845</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="2">
+        <v>10011</v>
+      </c>
+      <c r="L14" s="35">
+        <f>K14/J6</f>
+        <v>6.6918449197860967E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2141,8 +2199,15 @@
         <f t="shared" si="1"/>
         <v>1.8574459418471529</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="2">
+        <v>8919</v>
+      </c>
+      <c r="L15" s="35">
+        <f>K15/J6</f>
+        <v>5.9618983957219248E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
@@ -2169,8 +2234,15 @@
         <f t="shared" si="1"/>
         <v>1.0714277640838659</v>
       </c>
-    </row>
-    <row r="17" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="2">
+        <v>12104</v>
+      </c>
+      <c r="L16" s="35">
+        <f>K16/J6</f>
+        <v>8.0909090909090904E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
@@ -2197,8 +2269,15 @@
         <f t="shared" si="1"/>
         <v>0.62416093655543159</v>
       </c>
-    </row>
-    <row r="18" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="2">
+        <v>11831</v>
+      </c>
+      <c r="L17" s="35">
+        <f>K17/J6</f>
+        <v>7.9084224598930481E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
@@ -2225,8 +2304,9 @@
         <f t="shared" si="1"/>
         <v>0.35302976258633278</v>
       </c>
-    </row>
-    <row r="19" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
@@ -2253,8 +2333,9 @@
         <f t="shared" si="1"/>
         <v>0.18625255478617669</v>
       </c>
-    </row>
-    <row r="20" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L19" s="35"/>
+    </row>
+    <row r="20" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C20" s="2" t="s">
         <v>13</v>
       </c>
@@ -2281,8 +2362,15 @@
         <f t="shared" si="1"/>
         <v>0.10936278894891976</v>
       </c>
-    </row>
-    <row r="21" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="2">
+        <v>138846</v>
+      </c>
+      <c r="L20" s="35">
+        <f>K20/J6</f>
+        <v>9.2811497326203212E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
@@ -2309,8 +2397,15 @@
         <f t="shared" si="1"/>
         <v>4.3696793501415011E-2</v>
       </c>
-    </row>
-    <row r="22" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K21" s="2">
+        <v>149731</v>
+      </c>
+      <c r="L21" s="35">
+        <f>K21/J6</f>
+        <v>1.0008756684491979E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
@@ -2337,8 +2432,15 @@
         <f t="shared" si="1"/>
         <v>2.3708002345528723E-2</v>
       </c>
-    </row>
-    <row r="23" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K22" s="2">
+        <v>52721</v>
+      </c>
+      <c r="L22" s="35">
+        <f>K22/J6</f>
+        <v>3.5241310160427809E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="2" t="s">
         <v>25</v>
       </c>
@@ -2365,8 +2467,15 @@
         <f t="shared" si="1"/>
         <v>1.2056629429096967E-2</v>
       </c>
-    </row>
-    <row r="24" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K23" s="2">
+        <v>36657</v>
+      </c>
+      <c r="L23" s="35">
+        <f>K23/J6</f>
+        <v>2.4503342245989305E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
         <v>26</v>
       </c>
@@ -2393,27 +2502,28 @@
         <f t="shared" si="1"/>
         <v>6.5901617758925331E-3</v>
       </c>
-    </row>
-    <row r="25" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L24" s="35"/>
+    </row>
+    <row r="25" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
       <c r="G25" s="9"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="3:10" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
       <c r="G26" s="12"/>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C29" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
         <v>44</v>
       </c>
@@ -2421,7 +2531,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="3:10" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:12" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C31" s="3" t="s">
         <v>51</v>
       </c>
@@ -2429,7 +2539,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C33" s="18" t="s">
         <v>48</v>
@@ -2442,160 +2552,160 @@
     </row>
     <row r="35" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C35" s="18"/>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
     </row>
     <row r="36" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C36" s="18"/>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
     </row>
     <row r="37" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C37" s="18"/>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
     </row>
     <row r="38" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C38" s="18"/>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
     </row>
     <row r="39" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C39" s="18"/>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
     </row>
     <row r="40" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C40" s="18"/>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
     </row>
     <row r="41" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C41" s="18"/>
-      <c r="D41" s="33" t="s">
+      <c r="D41" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
     </row>
     <row r="42" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C42" s="18"/>
-      <c r="D42" s="33" t="s">
+      <c r="D42" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C43" s="18"/>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C44" s="18"/>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C45" s="18"/>
       <c r="D45" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
     </row>
     <row r="46" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C46" s="18"/>
-      <c r="D46" s="33" t="s">
+      <c r="D46" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
     </row>
     <row r="47" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C47" s="18"/>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
     </row>
     <row r="48" spans="3:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C48" s="18"/>
-      <c r="D48" s="33" t="s">
+      <c r="D48" s="31" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="49" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C49" s="18"/>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="31" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C50" s="18"/>
-      <c r="D50" s="33" t="s">
+      <c r="D50" s="31" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="51" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C51" s="18"/>
-      <c r="D51" s="33" t="s">
+      <c r="D51" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="52" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C52" s="18"/>
-      <c r="D52" s="33" t="s">
+      <c r="D52" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="53" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C53" s="18"/>
-      <c r="D53" s="33" t="s">
+      <c r="D53" s="31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C54" s="18"/>
-      <c r="D54" s="33" t="s">
+      <c r="D54" s="31" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2603,17 +2713,17 @@
       <c r="C55" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D55" s="33"/>
+      <c r="D55" s="31"/>
     </row>
     <row r="56" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C56" s="1"/>
-      <c r="D56" s="33" t="s">
+      <c r="D56" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C57" s="1"/>
-      <c r="D57" s="33" t="s">
+      <c r="D57" s="31" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2625,13 +2735,13 @@
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C59" s="1"/>
-      <c r="D59" s="33" t="s">
+      <c r="D59" s="31" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C60" s="1"/>
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="31" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2639,65 +2749,65 @@
       <c r="C61" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D61" s="33"/>
+      <c r="D61" s="31"/>
     </row>
     <row r="62" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C62" s="1"/>
-      <c r="D62" s="33" t="s">
+      <c r="D62" s="31" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="63" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C63" s="1"/>
-      <c r="D63" s="33" t="s">
+      <c r="D63" s="31" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="64" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C64" s="1"/>
-      <c r="D64" s="33" t="s">
+      <c r="D64" s="31" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C65" s="1"/>
-      <c r="D65" s="33" t="s">
+      <c r="D65" s="31" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C66" s="1"/>
-      <c r="D66" s="33" t="s">
+      <c r="D66" s="31" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="67" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C67" s="1"/>
-      <c r="D67" s="33" t="s">
+      <c r="D67" s="31" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="68" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C68" s="1"/>
-      <c r="D68" s="33" t="s">
+      <c r="D68" s="31" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C69" s="1"/>
-      <c r="D69" s="33" t="s">
+      <c r="D69" s="31" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="70" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C70" s="1"/>
-      <c r="D70" s="33" t="s">
+      <c r="D70" s="31" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71" s="1"/>
-      <c r="D71" s="33" t="s">
+      <c r="D71" s="31" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2705,41 +2815,41 @@
       <c r="C72" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D72" s="33"/>
+      <c r="D72" s="31"/>
     </row>
     <row r="73" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C73" s="1"/>
-      <c r="D73" s="33" t="s">
+      <c r="D73" s="31" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C74" s="18"/>
-      <c r="D74" s="33" t="s">
+      <c r="D74" s="31" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C75" s="18"/>
-      <c r="D75" s="33" t="s">
+      <c r="D75" s="31" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="76" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C76" s="18"/>
-      <c r="D76" s="33" t="s">
+      <c r="D76" s="31" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="77" spans="3:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C77" s="18"/>
-      <c r="D77" s="33" t="s">
+      <c r="D77" s="31" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C78" s="18"/>
-      <c r="D78" s="33" t="s">
+      <c r="D78" s="31" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>